<commit_message>
GDE-6723 - For Review
finalized codes for review
</commit_message>
<xml_diff>
--- a/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT02.xlsx
+++ b/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT02.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="1" activeTab="5" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UAT02_Runbook" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -24,7 +24,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -68,6 +68,18 @@
       <sz val="10"/>
       <u val="single"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -95,7 +107,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -142,11 +154,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF5B9BD5"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF5B9BD5"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF5B9BD5"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF5B9BD5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -199,6 +226,11 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="10" fontId="8" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1087,7 +1119,7 @@
   </sheetPr>
   <dimension ref="A1:EH14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
@@ -2609,8 +2641,8 @@
   </sheetPr>
   <dimension ref="A1:BD4"/>
   <sheetViews>
-    <sheetView topLeftCell="AV1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView topLeftCell="AP1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AS2" sqref="AS2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -2978,17 +3010,17 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>UAT2_25082020162712</t>
+          <t>UAT2_26082020103334</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>UAT225082020162713</t>
+          <t>UAT226082020103335</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>SF_08102019113147PBS</t>
+          <t>SF_26082020082952PCL</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
@@ -3031,9 +3063,9 @@
           <t>RTGS</t>
         </is>
       </c>
-      <c r="P2" s="1" t="inlineStr">
-        <is>
-          <t>%DBU</t>
+      <c r="P2" s="36" t="inlineStr">
+        <is>
+          <t>%AUSTCB001</t>
         </is>
       </c>
       <c r="Q2" s="1" t="inlineStr">
@@ -3178,7 +3210,7 @@
       </c>
       <c r="AS2" s="1" t="inlineStr">
         <is>
-          <t>COMMONWEALTH BANK AU-DBU</t>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
       <c r="AT2" s="1" t="inlineStr">
@@ -3224,7 +3256,7 @@
       </c>
       <c r="BC2" s="1" t="inlineStr">
         <is>
-          <t>Commonwealth Bank of Australia - DBU</t>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
       <c r="BD2" s="1" t="inlineStr">
@@ -3287,8 +3319,8 @@
   </sheetPr>
   <dimension ref="A1:AB4"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -3483,12 +3515,12 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>UAT2_25082020162712</t>
+          <t>UAT2_26082020103334</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>SF_08102019113147PBS</t>
+          <t>SF_26082020082952PCL</t>
         </is>
       </c>
       <c r="F2" s="29" t="inlineStr">
@@ -3538,7 +3570,7 @@
       </c>
       <c r="O2" s="29" t="inlineStr">
         <is>
-          <t>COMMONWEALTH BANK AU-DBU</t>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
       <c r="P2" s="29" t="inlineStr">
@@ -3563,7 +3595,7 @@
       </c>
       <c r="T2" s="14" t="inlineStr">
         <is>
-          <t>Commonwealth Bank Australia - DBU</t>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
       <c r="U2" s="14" t="inlineStr">
@@ -3625,7 +3657,7 @@
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>UAT2_25082020162712</t>
+          <t>UAT2_26082020103334</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
@@ -3680,7 +3712,7 @@
       </c>
       <c r="O3" s="29" t="inlineStr">
         <is>
-          <t>COMMONWEALTH BANK AU-DBU</t>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
       <c r="P3" s="29" t="inlineStr">
@@ -3705,7 +3737,7 @@
       </c>
       <c r="T3" s="14" t="inlineStr">
         <is>
-          <t>Commonwealth Bank Australia - DBU</t>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
       <c r="U3" s="14" t="inlineStr">
@@ -3767,7 +3799,7 @@
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>UAT2_25082020162712</t>
+          <t>UAT2_26082020103334</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr">
@@ -3822,7 +3854,7 @@
       </c>
       <c r="O4" s="29" t="inlineStr">
         <is>
-          <t>COMMONWEALTH BANK AU-DBU</t>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
       <c r="P4" s="29" t="inlineStr">
@@ -3847,7 +3879,7 @@
       </c>
       <c r="T4" s="14" t="inlineStr">
         <is>
-          <t>Commonwealth Bank Australia - DBU</t>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
       <c r="U4" s="14" t="inlineStr">
@@ -3906,8 +3938,8 @@
   </sheetPr>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -3989,7 +4021,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>SF_08102019113147PBS</t>
+          <t>SF_26082020082952PCL</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
@@ -4148,10 +4180,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AW5"/>
+  <dimension ref="A1:AX5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -4163,15 +4195,15 @@
     <col width="11" customWidth="1" style="1" min="5" max="5"/>
     <col width="17.42578125" customWidth="1" style="1" min="6" max="6"/>
     <col width="16.140625" customWidth="1" style="1" min="7" max="7"/>
-    <col width="17.5703125" customWidth="1" style="1" min="8" max="8"/>
-    <col width="21.42578125" customWidth="1" style="1" min="9" max="9"/>
-    <col width="23.5703125" customWidth="1" style="1" min="10" max="10"/>
-    <col width="18.7109375" customWidth="1" style="1" min="11" max="11"/>
-    <col width="18.28515625" customWidth="1" style="1" min="12" max="12"/>
-    <col width="23.85546875" customWidth="1" style="1" min="13" max="13"/>
-    <col width="24" customWidth="1" style="1" min="14" max="14"/>
-    <col width="22.85546875" customWidth="1" style="1" min="15" max="15"/>
-    <col width="22.140625" customWidth="1" style="1" min="16" max="16"/>
+    <col width="17.5703125" customWidth="1" style="1" min="8" max="9"/>
+    <col width="21.42578125" customWidth="1" style="1" min="10" max="10"/>
+    <col width="23.5703125" customWidth="1" style="1" min="11" max="11"/>
+    <col width="18.7109375" customWidth="1" style="1" min="12" max="12"/>
+    <col width="18.28515625" customWidth="1" style="1" min="13" max="13"/>
+    <col width="23.85546875" customWidth="1" style="1" min="14" max="14"/>
+    <col width="24" customWidth="1" style="1" min="15" max="15"/>
+    <col width="22.85546875" customWidth="1" style="1" min="16" max="16"/>
+    <col width="22.140625" customWidth="1" style="1" min="17" max="17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="5">
@@ -4217,46 +4249,51 @@
       </c>
       <c r="I1" s="5" t="inlineStr">
         <is>
+          <t>Loan_AllInRate</t>
+        </is>
+      </c>
+      <c r="J1" s="5" t="inlineStr">
+        <is>
           <t>Outstanding_Currency</t>
         </is>
       </c>
-      <c r="J1" s="5" t="inlineStr">
+      <c r="K1" s="5" t="inlineStr">
         <is>
           <t>Loan_RequestedAmount</t>
         </is>
       </c>
-      <c r="K1" s="5" t="inlineStr">
+      <c r="L1" s="5" t="inlineStr">
         <is>
           <t>Loan_EffectiveDate</t>
         </is>
       </c>
-      <c r="L1" s="5" t="inlineStr">
+      <c r="M1" s="5" t="inlineStr">
         <is>
           <t>Loan_MaturityDate</t>
         </is>
       </c>
-      <c r="M1" s="5" t="inlineStr">
+      <c r="N1" s="5" t="inlineStr">
         <is>
           <t>Loan_IntCycleFrequency</t>
         </is>
       </c>
-      <c r="N1" s="5" t="inlineStr">
+      <c r="O1" s="5" t="inlineStr">
         <is>
           <t>Loan_BorrowerBaseRate</t>
         </is>
       </c>
-      <c r="O1" s="21" t="inlineStr">
+      <c r="P1" s="21" t="inlineStr">
         <is>
           <t>Remittance_Description</t>
         </is>
       </c>
-      <c r="P1" s="21" t="inlineStr">
+      <c r="Q1" s="21" t="inlineStr">
         <is>
           <t>Remittance_Instruction</t>
         </is>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" s="1" t="inlineStr">
         <is>
           <t>1</t>
@@ -4269,12 +4306,12 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>UAT2_25082020162712</t>
+          <t>UAT2_26082020103334</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>SF_08102019113147PBS</t>
+          <t>SF_26082020082952PCL</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
@@ -4297,103 +4334,106 @@
           <t>Loan</t>
         </is>
       </c>
-      <c r="I2" s="1" t="inlineStr">
+      <c r="I2" s="37" t="n">
+        <v>0.0413</v>
+      </c>
+      <c r="J2" s="1" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="J2" s="29" t="inlineStr">
+      <c r="K2" s="29" t="inlineStr">
         <is>
           <t>991,977.80</t>
         </is>
       </c>
-      <c r="K2" s="1" t="inlineStr">
+      <c r="L2" s="1" t="inlineStr">
         <is>
           <t>27-Sep-2018</t>
         </is>
       </c>
-      <c r="L2" s="1" t="inlineStr">
+      <c r="M2" s="1" t="inlineStr">
         <is>
           <t>28-Jun-2038</t>
         </is>
       </c>
-      <c r="M2" s="1" t="inlineStr">
+      <c r="N2" s="1" t="inlineStr">
         <is>
           <t>Quarterly</t>
         </is>
       </c>
-      <c r="N2" s="1" t="inlineStr">
+      <c r="O2" s="1" t="inlineStr">
         <is>
           <t>2.79</t>
         </is>
       </c>
-      <c r="O2" s="1" t="inlineStr">
+      <c r="P2" s="1" t="inlineStr">
         <is>
           <t>RTGS1- TO CUSTOMER</t>
         </is>
       </c>
-      <c r="P2" s="1" t="inlineStr">
+      <c r="Q2" s="1" t="inlineStr">
         <is>
           <t>RTGS</t>
         </is>
       </c>
-      <c r="Q2" s="1" t="inlineStr">
+      <c r="R2" s="1" t="inlineStr">
         <is>
           <t>1.34</t>
         </is>
       </c>
-      <c r="T2" s="1" t="inlineStr">
+      <c r="U2" s="1" t="inlineStr">
         <is>
           <t>1.34</t>
         </is>
       </c>
-      <c r="W2" s="1" t="inlineStr">
+      <c r="X2" s="1" t="inlineStr">
         <is>
           <t>1.34</t>
         </is>
       </c>
-      <c r="Z2" s="1" t="inlineStr">
+      <c r="AA2" s="1" t="inlineStr">
         <is>
           <t>1.34</t>
         </is>
       </c>
-      <c r="AC2" s="1" t="inlineStr">
+      <c r="AD2" s="1" t="inlineStr">
         <is>
           <t>1.34</t>
         </is>
       </c>
-      <c r="AF2" s="1" t="inlineStr">
+      <c r="AG2" s="1" t="inlineStr">
         <is>
           <t>1.34</t>
         </is>
       </c>
-      <c r="AI2" s="1" t="inlineStr">
+      <c r="AJ2" s="1" t="inlineStr">
         <is>
           <t>1.34</t>
         </is>
       </c>
-      <c r="AL2" s="1" t="inlineStr">
+      <c r="AM2" s="1" t="inlineStr">
         <is>
           <t>1.34</t>
         </is>
       </c>
-      <c r="AO2" s="1" t="inlineStr">
+      <c r="AP2" s="1" t="inlineStr">
         <is>
           <t>1.34</t>
         </is>
       </c>
-      <c r="AR2" s="1" t="inlineStr">
+      <c r="AS2" s="1" t="inlineStr">
         <is>
           <t>1.34</t>
         </is>
       </c>
-      <c r="AU2" s="1" t="inlineStr">
+      <c r="AV2" s="1" t="inlineStr">
         <is>
           <t>1.34</t>
         </is>
       </c>
     </row>
-    <row r="3">
+    <row r="3" ht="15" customHeight="1">
       <c r="A3" s="1" t="inlineStr">
         <is>
           <t>2</t>
@@ -4406,7 +4446,7 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>UAT2_25082020162712</t>
+          <t>UAT2_26082020103334</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
@@ -4434,103 +4474,106 @@
           <t>Loan</t>
         </is>
       </c>
-      <c r="I3" s="1" t="inlineStr">
+      <c r="I3" s="37" t="n">
+        <v>0.0413</v>
+      </c>
+      <c r="J3" s="1" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="J3" s="29" t="inlineStr">
+      <c r="K3" s="29" t="inlineStr">
         <is>
           <t>979,383.39</t>
         </is>
       </c>
-      <c r="K3" s="1" t="inlineStr">
+      <c r="L3" s="1" t="inlineStr">
         <is>
           <t>27-Sep-2018</t>
         </is>
       </c>
-      <c r="L3" s="1" t="inlineStr">
+      <c r="M3" s="1" t="inlineStr">
         <is>
           <t>27-Jun-2038</t>
         </is>
       </c>
-      <c r="M3" s="1" t="inlineStr">
+      <c r="N3" s="1" t="inlineStr">
         <is>
           <t>Quarterly</t>
         </is>
       </c>
-      <c r="N3" s="1" t="inlineStr">
+      <c r="O3" s="1" t="inlineStr">
         <is>
           <t>2.51</t>
         </is>
       </c>
-      <c r="O3" s="1" t="inlineStr">
+      <c r="P3" s="1" t="inlineStr">
         <is>
           <t>RTGS1- TO CUSTOMER</t>
         </is>
       </c>
-      <c r="P3" s="1" t="inlineStr">
+      <c r="Q3" s="1" t="inlineStr">
         <is>
           <t>RTGS</t>
         </is>
       </c>
-      <c r="R3" s="1" t="inlineStr">
+      <c r="S3" s="1" t="inlineStr">
         <is>
           <t>1.27</t>
         </is>
       </c>
-      <c r="U3" s="1" t="inlineStr">
+      <c r="V3" s="1" t="inlineStr">
         <is>
           <t>1.27</t>
         </is>
       </c>
-      <c r="X3" s="1" t="inlineStr">
+      <c r="Y3" s="1" t="inlineStr">
         <is>
           <t>1.27</t>
         </is>
       </c>
-      <c r="AA3" s="1" t="inlineStr">
+      <c r="AB3" s="1" t="inlineStr">
         <is>
           <t>1.27</t>
         </is>
       </c>
-      <c r="AD3" s="1" t="inlineStr">
+      <c r="AE3" s="1" t="inlineStr">
         <is>
           <t>1.27</t>
         </is>
       </c>
-      <c r="AG3" s="1" t="inlineStr">
+      <c r="AH3" s="1" t="inlineStr">
         <is>
           <t>1.27</t>
         </is>
       </c>
-      <c r="AJ3" s="1" t="inlineStr">
+      <c r="AK3" s="1" t="inlineStr">
         <is>
           <t>1.27</t>
         </is>
       </c>
-      <c r="AM3" s="1" t="inlineStr">
+      <c r="AN3" s="1" t="inlineStr">
         <is>
           <t>1.27</t>
         </is>
       </c>
-      <c r="AP3" s="1" t="inlineStr">
+      <c r="AQ3" s="1" t="inlineStr">
         <is>
           <t>1.27</t>
         </is>
       </c>
-      <c r="AS3" s="1" t="inlineStr">
+      <c r="AT3" s="1" t="inlineStr">
         <is>
           <t>1.27</t>
         </is>
       </c>
-      <c r="AV3" s="1" t="inlineStr">
+      <c r="AW3" s="1" t="inlineStr">
         <is>
           <t>1.27</t>
         </is>
       </c>
     </row>
-    <row r="4">
+    <row r="4" ht="15" customHeight="1">
       <c r="A4" s="1" t="inlineStr">
         <is>
           <t>3</t>
@@ -4543,7 +4586,7 @@
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>UAT2_25082020162712</t>
+          <t>UAT2_26082020103334</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
@@ -4571,97 +4614,100 @@
           <t>Loan</t>
         </is>
       </c>
-      <c r="I4" s="1" t="inlineStr">
+      <c r="I4" s="38" t="n">
+        <v>0.0413</v>
+      </c>
+      <c r="J4" s="1" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="J4" s="29" t="inlineStr">
+      <c r="K4" s="29" t="inlineStr">
         <is>
           <t>2,479,944.52</t>
         </is>
       </c>
-      <c r="K4" s="1" t="inlineStr">
+      <c r="L4" s="1" t="inlineStr">
         <is>
           <t>27-Sep-2018</t>
         </is>
       </c>
-      <c r="L4" s="1" t="inlineStr">
+      <c r="M4" s="1" t="inlineStr">
         <is>
           <t>28-Jun-2038</t>
         </is>
       </c>
-      <c r="M4" s="1" t="inlineStr">
+      <c r="N4" s="1" t="inlineStr">
         <is>
           <t>Quarterly</t>
         </is>
       </c>
-      <c r="N4" s="1" t="inlineStr">
+      <c r="O4" s="1" t="inlineStr">
         <is>
           <t>2.79</t>
         </is>
       </c>
-      <c r="O4" s="1" t="inlineStr">
+      <c r="P4" s="1" t="inlineStr">
         <is>
           <t>RTGS1- TO CUSTOMER</t>
         </is>
       </c>
-      <c r="P4" s="1" t="inlineStr">
+      <c r="Q4" s="1" t="inlineStr">
         <is>
           <t>RTGS</t>
         </is>
       </c>
-      <c r="S4" s="1" t="inlineStr">
+      <c r="T4" s="1" t="inlineStr">
         <is>
           <t>1.34</t>
         </is>
       </c>
-      <c r="V4" s="1" t="inlineStr">
+      <c r="W4" s="1" t="inlineStr">
         <is>
           <t>1.34</t>
         </is>
       </c>
-      <c r="Y4" s="1" t="inlineStr">
+      <c r="Z4" s="1" t="inlineStr">
         <is>
           <t>1.34</t>
         </is>
       </c>
-      <c r="AB4" s="1" t="inlineStr">
+      <c r="AC4" s="1" t="inlineStr">
         <is>
           <t>1.34</t>
         </is>
       </c>
-      <c r="AE4" s="1" t="inlineStr">
+      <c r="AF4" s="1" t="inlineStr">
         <is>
           <t>1.34</t>
         </is>
       </c>
-      <c r="AH4" s="1" t="inlineStr">
+      <c r="AI4" s="1" t="inlineStr">
         <is>
           <t>1.34</t>
         </is>
       </c>
-      <c r="AK4" s="1" t="inlineStr">
+      <c r="AL4" s="1" t="inlineStr">
         <is>
           <t>1.34</t>
         </is>
       </c>
-      <c r="AN4" s="1" t="inlineStr">
+      <c r="AO4" s="1" t="inlineStr">
         <is>
           <t>1.34</t>
         </is>
       </c>
-      <c r="AQ4" s="1" t="inlineStr">
+      <c r="AR4" s="1" t="inlineStr">
         <is>
           <t>1.34</t>
         </is>
       </c>
-      <c r="AT4" s="1" t="inlineStr">
+      <c r="AU4" s="1" t="inlineStr">
         <is>
           <t>1.34</t>
         </is>
       </c>
-      <c r="AW4" s="1" t="inlineStr">
+      <c r="AX4" s="1" t="inlineStr">
         <is>
           <t>1.34</t>
         </is>
@@ -4670,7 +4716,7 @@
     <row r="5">
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>UAT2_25082020162712</t>
+          <t>UAT2_26082020103334</t>
         </is>
       </c>
       <c r="F5" s="1" t="inlineStr">
@@ -4678,7 +4724,7 @@
           <t>BE Pty Ltd 08202066</t>
         </is>
       </c>
-      <c r="O5" s="1" t="inlineStr">
+      <c r="P5" s="1" t="inlineStr">
         <is>
           <t>RTGS1- TO CUSTOMER</t>
         </is>
@@ -4700,7 +4746,7 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -4830,12 +4876,12 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>UAT2_25082020162712</t>
+          <t>UAT2_26082020103334</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>SF_08102019113147PBS</t>
+          <t>SF_26082020082952PCL</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
@@ -4922,7 +4968,7 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>UAT2_25082020162712</t>
+          <t>UAT2_26082020103334</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
@@ -5014,7 +5060,7 @@
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>UAT2_25082020162712</t>
+          <t>UAT2_26082020103334</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
@@ -5076,7 +5122,7 @@
     <row r="5">
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>UAT2_25082020162712</t>
+          <t>UAT2_26082020103334</t>
         </is>
       </c>
       <c r="G5" s="1" t="inlineStr">

</xml_diff>

<commit_message>
GDE-6786 latest dev merged with branch
</commit_message>
<xml_diff>
--- a/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT02.xlsx
+++ b/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT02.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="1" activeTab="5" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UAT02_Runbook" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -62,22 +62,20 @@
       <u val="single"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <color indexed="30"/>
-      <sz val="10"/>
-      <u val="single"/>
-    </font>
-    <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color rgb="FF000000"/>
       <sz val="11"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <sz val="10"/>
+    </font>
+    <font>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF444444"/>
       <sz val="11"/>
     </font>
   </fonts>
@@ -195,7 +193,6 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -229,8 +226,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="10" fontId="8" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,7 +541,7 @@
   <dimension ref="A1:CP3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="U35" sqref="U35"/>
     </sheetView>
   </sheetViews>
@@ -1119,8 +1117,8 @@
   </sheetPr>
   <dimension ref="A1:EH14"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -2053,9 +2051,9 @@
           <t>CBA Email with PDF Attachment</t>
         </is>
       </c>
-      <c r="V2" s="13" t="inlineStr">
-        <is>
-          <t>Samiha.Bakhtiar@cba.com.au</t>
+      <c r="V2" s="38" t="inlineStr">
+        <is>
+          <t>billy.elliot@danceswithwolves.com</t>
         </is>
       </c>
       <c r="W2" s="7" t="inlineStr">
@@ -2063,27 +2061,27 @@
           <t>Elliot</t>
         </is>
       </c>
-      <c r="X2" s="14" t="inlineStr">
+      <c r="X2" s="13" t="inlineStr">
         <is>
           <t>OFF</t>
         </is>
       </c>
-      <c r="Y2" s="14" t="inlineStr">
+      <c r="Y2" s="13" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="Z2" s="14" t="inlineStr">
+      <c r="Z2" s="13" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="AA2" s="14" t="inlineStr">
+      <c r="AA2" s="13" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="AB2" s="14" t="inlineStr">
+      <c r="AB2" s="13" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
@@ -2193,7 +2191,7 @@
           <t>Australia</t>
         </is>
       </c>
-      <c r="AY2" s="16" t="inlineStr">
+      <c r="AY2" s="15" t="inlineStr">
         <is>
           <t xml:space="preserve">412345678
  </t>
@@ -2294,17 +2292,17 @@
           <t>CBA Domestic Account</t>
         </is>
       </c>
-      <c r="BS2" s="14" t="inlineStr">
+      <c r="BS2" s="13" t="inlineStr">
         <is>
           <t>1020188515</t>
         </is>
       </c>
-      <c r="BT2" s="14" t="inlineStr">
+      <c r="BT2" s="13" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="BU2" s="14" t="inlineStr">
+      <c r="BU2" s="13" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
@@ -2339,32 +2337,32 @@
           <t>IMT-USD2519</t>
         </is>
       </c>
-      <c r="CB2" s="14" t="inlineStr">
+      <c r="CB2" s="13" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="CC2" s="14" t="inlineStr">
+      <c r="CC2" s="13" t="inlineStr">
         <is>
           <t>MT103</t>
         </is>
       </c>
-      <c r="CD2" s="14" t="inlineStr">
+      <c r="CD2" s="13" t="inlineStr">
         <is>
           <t>Ordering Customer</t>
         </is>
       </c>
-      <c r="CE2" s="14" t="inlineStr">
+      <c r="CE2" s="13" t="inlineStr">
         <is>
           <t>Credit transfer - Service Level: Standard</t>
         </is>
       </c>
-      <c r="CF2" s="14" t="inlineStr">
+      <c r="CF2" s="13" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="CG2" s="14" t="inlineStr">
+      <c r="CG2" s="13" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
@@ -2399,47 +2397,47 @@
           <t>14162984821</t>
         </is>
       </c>
-      <c r="CN2" s="15" t="inlineStr">
+      <c r="CN2" s="14" t="inlineStr">
         <is>
           <t>Internal Rating</t>
         </is>
       </c>
-      <c r="CO2" s="15" t="inlineStr">
+      <c r="CO2" s="14" t="inlineStr">
         <is>
           <t>D1 Good</t>
         </is>
       </c>
-      <c r="CP2" s="15" t="inlineStr">
+      <c r="CP2" s="14" t="inlineStr">
         <is>
           <t>100</t>
         </is>
       </c>
-      <c r="CQ2" s="15" t="inlineStr">
+      <c r="CQ2" s="14" t="inlineStr">
         <is>
           <t>Standard &amp; Poors</t>
         </is>
       </c>
-      <c r="CR2" s="15" t="inlineStr">
+      <c r="CR2" s="14" t="inlineStr">
         <is>
           <t>BBB+</t>
         </is>
       </c>
-      <c r="CS2" s="15" t="inlineStr">
+      <c r="CS2" s="14" t="inlineStr">
         <is>
           <t>Moody's Investor Services Inc</t>
         </is>
       </c>
-      <c r="CT2" s="15" t="inlineStr">
+      <c r="CT2" s="14" t="inlineStr">
         <is>
           <t>Aa2</t>
         </is>
       </c>
-      <c r="CU2" s="15" t="inlineStr">
+      <c r="CU2" s="14" t="inlineStr">
         <is>
           <t>Fitch</t>
         </is>
       </c>
-      <c r="CV2" s="15" t="inlineStr">
+      <c r="CV2" s="14" t="inlineStr">
         <is>
           <t>A+</t>
         </is>
@@ -2449,17 +2447,17 @@
           <t>LEGAL ADDRESS</t>
         </is>
       </c>
-      <c r="CX2" s="15" t="inlineStr">
+      <c r="CX2" s="14" t="inlineStr">
         <is>
           <t>PO Box 861</t>
         </is>
       </c>
-      <c r="CY2" s="15" t="inlineStr">
+      <c r="CY2" s="14" t="inlineStr">
         <is>
           <t>Almond, Victoria 3211</t>
         </is>
       </c>
-      <c r="CZ2" s="16" t="inlineStr">
+      <c r="CZ2" s="15" t="inlineStr">
         <is>
           <t>03 5029 9445</t>
         </is>
@@ -2469,46 +2467,46 @@
           <t>Account With Institution</t>
         </is>
       </c>
-      <c r="DB2" s="17" t="inlineStr">
+      <c r="DB2" s="16" t="inlineStr">
         <is>
           <t>Beneficiary Customer</t>
         </is>
       </c>
-      <c r="DC2" s="17" t="inlineStr">
+      <c r="DC2" s="16" t="inlineStr">
         <is>
           <t>Ordering Customer</t>
         </is>
       </c>
-      <c r="DD2" s="17" t="inlineStr">
+      <c r="DD2" s="16" t="inlineStr">
         <is>
           <t>Account With Institution</t>
         </is>
       </c>
-      <c r="DE2" s="17" t="inlineStr">
+      <c r="DE2" s="16" t="inlineStr">
         <is>
           <t>NATAAU33033</t>
         </is>
       </c>
-      <c r="DF2" s="14" t="inlineStr">
+      <c r="DF2" s="13" t="inlineStr">
         <is>
           <t>NATIONAL AUSTRALIA BANK LIMITED</t>
         </is>
       </c>
-      <c r="DG2" s="14" t="n"/>
-      <c r="DH2" s="14" t="inlineStr">
+      <c r="DG2" s="13" t="n"/>
+      <c r="DH2" s="13" t="inlineStr">
         <is>
           <t>//AU082674</t>
         </is>
       </c>
-      <c r="DI2" s="17" t="n"/>
-      <c r="DJ2" s="14" t="n"/>
-      <c r="DK2" s="14" t="n"/>
+      <c r="DI2" s="16" t="n"/>
+      <c r="DJ2" s="13" t="n"/>
+      <c r="DK2" s="13" t="n"/>
       <c r="DL2" s="1" t="inlineStr">
         <is>
           <t>BE Pty Ltd as trustee for the Dances With Wolves Family Trust</t>
         </is>
       </c>
-      <c r="DM2" s="14" t="inlineStr">
+      <c r="DM2" s="13" t="inlineStr">
         <is>
           <t>/509748214</t>
         </is>
@@ -2518,98 +2516,98 @@
           <t>BE Pty Ltd as trustee for the Dances With Wolves Family Trust</t>
         </is>
       </c>
-      <c r="DO2" s="14" t="n"/>
-      <c r="DP2" s="14" t="inlineStr">
+      <c r="DO2" s="13" t="n"/>
+      <c r="DP2" s="13" t="inlineStr">
         <is>
           <t>03-Jan-2019</t>
         </is>
       </c>
-      <c r="DQ2" s="18" t="inlineStr">
+      <c r="DQ2" s="17" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="DR2" s="14" t="inlineStr">
+      <c r="DR2" s="13" t="inlineStr">
         <is>
           <t>03-Jan-2019</t>
         </is>
       </c>
-      <c r="DS2" s="14" t="inlineStr">
+      <c r="DS2" s="13" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="DT2" s="14" t="inlineStr">
+      <c r="DT2" s="13" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="DU2" s="14" t="inlineStr">
+      <c r="DU2" s="13" t="inlineStr">
         <is>
           <t>OFF</t>
         </is>
       </c>
-      <c r="DV2" s="14" t="inlineStr">
+      <c r="DV2" s="13" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="DW2" s="14" t="inlineStr">
+      <c r="DW2" s="13" t="inlineStr">
         <is>
           <t xml:space="preserve">ON </t>
         </is>
       </c>
-      <c r="DX2" s="14" t="inlineStr">
+      <c r="DX2" s="13" t="inlineStr">
         <is>
           <t>OFF</t>
         </is>
       </c>
-      <c r="DY2" s="14" t="inlineStr">
+      <c r="DY2" s="13" t="inlineStr">
         <is>
           <t>OFF</t>
         </is>
       </c>
-      <c r="DZ2" s="14" t="inlineStr">
+      <c r="DZ2" s="13" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="EA2" s="14" t="inlineStr">
+      <c r="EA2" s="13" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="EB2" s="14" t="inlineStr">
+      <c r="EB2" s="13" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="EC2" s="14" t="inlineStr">
+      <c r="EC2" s="13" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="ED2" s="14" t="inlineStr">
+      <c r="ED2" s="13" t="inlineStr">
         <is>
           <t>OFF</t>
         </is>
       </c>
-      <c r="EE2" s="14" t="inlineStr">
+      <c r="EE2" s="13" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="EF2" s="14" t="inlineStr">
+      <c r="EF2" s="13" t="inlineStr">
         <is>
           <t>RTGS</t>
         </is>
       </c>
-      <c r="EG2" s="19" t="inlineStr">
+      <c r="EG2" s="18" t="inlineStr">
         <is>
           <t>Account Name: BE Pty Ltd as trustee for the Dances With Wolves Family Trust Account Number: 082674 50974821</t>
         </is>
       </c>
-      <c r="EH2" s="19" t="inlineStr">
+      <c r="EH2" s="18" t="inlineStr">
         <is>
           <t>Account Name:
 Account Number:</t>
@@ -2624,7 +2622,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="AM14" s="20" t="n"/>
+      <c r="AM14" s="19" t="n"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
@@ -2726,17 +2724,17 @@
           <t>Deal_AliasPrefix</t>
         </is>
       </c>
-      <c r="E1" s="21" t="inlineStr">
+      <c r="E1" s="20" t="inlineStr">
         <is>
           <t>Deal_Name</t>
         </is>
       </c>
-      <c r="F1" s="21" t="inlineStr">
+      <c r="F1" s="20" t="inlineStr">
         <is>
           <t>Deal_Alias</t>
         </is>
       </c>
-      <c r="G1" s="21" t="inlineStr">
+      <c r="G1" s="20" t="inlineStr">
         <is>
           <t>Facility_Name</t>
         </is>
@@ -2751,12 +2749,12 @@
           <t>Deal_SalesGroup</t>
         </is>
       </c>
-      <c r="J1" s="21" t="inlineStr">
+      <c r="J1" s="20" t="inlineStr">
         <is>
           <t>Borrower_ShortName</t>
         </is>
       </c>
-      <c r="K1" s="21" t="inlineStr">
+      <c r="K1" s="20" t="inlineStr">
         <is>
           <t>Borrower_Location</t>
         </is>
@@ -2966,7 +2964,7 @@
           <t>Primary_SGRIMethod</t>
         </is>
       </c>
-      <c r="BA1" s="21" t="inlineStr">
+      <c r="BA1" s="20" t="inlineStr">
         <is>
           <t>PrimaryFacility_Allocation</t>
         </is>
@@ -3010,17 +3008,17 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>UAT2_26082020103334</t>
+          <t>UAT2_27082020084411</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>UAT226082020103335</t>
+          <t>UAT227082020084411</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>SF_26082020082952PCL</t>
+          <t>SF_27082020085203AGP</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
@@ -3063,7 +3061,7 @@
           <t>RTGS</t>
         </is>
       </c>
-      <c r="P2" s="36" t="inlineStr">
+      <c r="P2" s="35" t="inlineStr">
         <is>
           <t>%AUSTCB001</t>
         </is>
@@ -3118,7 +3116,7 @@
           <t>26-Jun-2018</t>
         </is>
       </c>
-      <c r="AA2" s="22" t="inlineStr">
+      <c r="AA2" s="21" t="inlineStr">
         <is>
           <t>4,500,000.00</t>
         </is>
@@ -3273,7 +3271,7 @@
       </c>
       <c r="G3" s="1" t="inlineStr">
         <is>
-          <t>GF_08102019113812UHP</t>
+          <t>GF_27082020085831GAV</t>
         </is>
       </c>
       <c r="AD3" s="1" t="inlineStr">
@@ -3319,8 +3317,8 @@
   </sheetPr>
   <dimension ref="A1:AB4"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -3339,14 +3337,14 @@
     <col width="18.7109375" customWidth="1" style="1" min="12" max="12"/>
     <col width="20.28515625" customWidth="1" style="1" min="13" max="13"/>
     <col width="23.140625" customWidth="1" style="1" min="14" max="14"/>
-    <col width="31.28515625" customWidth="1" style="1" min="15" max="15"/>
+    <col width="36.28515625" bestFit="1" customWidth="1" style="1" min="15" max="15"/>
     <col width="16.85546875" customWidth="1" style="1" min="16" max="16"/>
     <col width="21.7109375" customWidth="1" style="1" min="17" max="17"/>
     <col width="25.5703125" customWidth="1" style="1" min="18" max="18"/>
     <col width="19.42578125" customWidth="1" style="1" min="19" max="19"/>
     <col width="32.7109375" customWidth="1" style="1" min="20" max="20"/>
     <col width="21" customWidth="1" style="1" min="21" max="21"/>
-    <col width="17.42578125" customWidth="1" style="1" min="22" max="22"/>
+    <col width="20.42578125" bestFit="1" customWidth="1" style="1" min="22" max="22"/>
     <col width="18.85546875" customWidth="1" style="1" min="23" max="23"/>
     <col width="24.7109375" customWidth="1" style="1" min="24" max="24"/>
     <col width="25.5703125" customWidth="1" style="1" min="25" max="25"/>
@@ -3355,451 +3353,451 @@
     <col width="19.42578125" customWidth="1" style="1" min="28" max="28"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.5" customFormat="1" customHeight="1" s="23" thickBot="1">
-      <c r="A1" s="24" t="inlineStr">
+    <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22" thickBot="1">
+      <c r="A1" s="23" t="inlineStr">
         <is>
           <t>rowid</t>
         </is>
       </c>
-      <c r="B1" s="24" t="inlineStr">
+      <c r="B1" s="23" t="inlineStr">
         <is>
           <t>Test_Case</t>
         </is>
       </c>
-      <c r="C1" s="25" t="inlineStr">
+      <c r="C1" s="24" t="inlineStr">
         <is>
           <t>Facility_NamePrefix</t>
         </is>
       </c>
-      <c r="D1" s="26" t="inlineStr">
+      <c r="D1" s="25" t="inlineStr">
         <is>
           <t>Deal_Name</t>
         </is>
       </c>
-      <c r="E1" s="26" t="inlineStr">
+      <c r="E1" s="25" t="inlineStr">
         <is>
           <t>Facility_Name</t>
         </is>
       </c>
-      <c r="F1" s="23" t="inlineStr">
+      <c r="F1" s="22" t="inlineStr">
         <is>
           <t>Deal_Currency</t>
         </is>
       </c>
-      <c r="G1" s="23" t="inlineStr">
+      <c r="G1" s="22" t="inlineStr">
         <is>
           <t>Facility_Type</t>
         </is>
       </c>
-      <c r="H1" s="23" t="inlineStr">
+      <c r="H1" s="22" t="inlineStr">
         <is>
           <t>Facility_ProposedCmtAmt</t>
         </is>
       </c>
-      <c r="I1" s="23" t="inlineStr">
+      <c r="I1" s="22" t="inlineStr">
         <is>
           <t>Facility_Currency</t>
         </is>
       </c>
-      <c r="J1" s="23" t="inlineStr">
+      <c r="J1" s="22" t="inlineStr">
         <is>
           <t>Facility_AgreementDate</t>
         </is>
       </c>
-      <c r="K1" s="23" t="inlineStr">
+      <c r="K1" s="22" t="inlineStr">
         <is>
           <t>Facility_EffectiveDate</t>
         </is>
       </c>
-      <c r="L1" s="23" t="inlineStr">
+      <c r="L1" s="22" t="inlineStr">
         <is>
           <t>Facility_ExpiryDate</t>
         </is>
       </c>
-      <c r="M1" s="23" t="inlineStr">
+      <c r="M1" s="22" t="inlineStr">
         <is>
           <t>Facility_MaturityDate</t>
         </is>
       </c>
-      <c r="N1" s="23" t="inlineStr">
+      <c r="N1" s="22" t="inlineStr">
         <is>
           <t>Facility_ServicingGroup</t>
         </is>
       </c>
-      <c r="O1" s="27" t="inlineStr">
+      <c r="O1" s="26" t="inlineStr">
         <is>
           <t>Facility_Customer</t>
         </is>
       </c>
-      <c r="P1" s="27" t="inlineStr">
+      <c r="P1" s="26" t="inlineStr">
         <is>
           <t>Facility_RiskType</t>
         </is>
       </c>
-      <c r="Q1" s="27" t="inlineStr">
+      <c r="Q1" s="26" t="inlineStr">
         <is>
           <t>Facility_RiskTypeLimit</t>
         </is>
       </c>
-      <c r="R1" s="27" t="inlineStr">
+      <c r="R1" s="26" t="inlineStr">
         <is>
           <t>Facility_LoanPurposeType</t>
         </is>
       </c>
-      <c r="S1" s="27" t="inlineStr">
+      <c r="S1" s="26" t="inlineStr">
         <is>
           <t>Facility_GlobalLimit</t>
         </is>
       </c>
-      <c r="T1" s="27" t="inlineStr">
+      <c r="T1" s="26" t="inlineStr">
         <is>
           <t>Facility_CustomerServicingGroup</t>
         </is>
       </c>
-      <c r="U1" s="27" t="inlineStr">
+      <c r="U1" s="26" t="inlineStr">
         <is>
           <t>Facility_SGLocation</t>
         </is>
       </c>
-      <c r="V1" s="28" t="inlineStr">
+      <c r="V1" s="27" t="inlineStr">
         <is>
           <t>Facility_Borrower</t>
         </is>
       </c>
-      <c r="W1" s="27" t="inlineStr">
+      <c r="W1" s="26" t="inlineStr">
         <is>
           <t>Borrower_Currency</t>
         </is>
       </c>
-      <c r="X1" s="27" t="inlineStr">
+      <c r="X1" s="26" t="inlineStr">
         <is>
           <t>Facility_BorrowerMaturity</t>
         </is>
       </c>
-      <c r="Y1" s="27" t="inlineStr">
+      <c r="Y1" s="26" t="inlineStr">
         <is>
           <t>Facility_BorrowerSGName</t>
         </is>
       </c>
-      <c r="Z1" s="27" t="inlineStr">
+      <c r="Z1" s="26" t="inlineStr">
         <is>
           <t>Facility_BorrowerPercent</t>
         </is>
       </c>
-      <c r="AA1" s="27" t="inlineStr">
+      <c r="AA1" s="26" t="inlineStr">
         <is>
           <t>CurrencyLimit</t>
         </is>
       </c>
-      <c r="AB1" s="27" t="inlineStr">
+      <c r="AB1" s="26" t="inlineStr">
         <is>
           <t>Facility_GlobalLimit</t>
         </is>
       </c>
     </row>
-    <row r="2" customFormat="1" s="14">
-      <c r="A2" s="14" t="inlineStr">
+    <row r="2" customFormat="1" s="13">
+      <c r="A2" s="13" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="B2" s="14" t="inlineStr">
+      <c r="B2" s="13" t="inlineStr">
         <is>
           <t>CBA_UAT_02</t>
         </is>
       </c>
-      <c r="C2" s="14" t="inlineStr">
+      <c r="C2" s="13" t="inlineStr">
         <is>
           <t>SF_</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>UAT2_26082020103334</t>
+          <t>UAT2_27082020084411</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>SF_26082020082952PCL</t>
-        </is>
-      </c>
-      <c r="F2" s="29" t="inlineStr">
+          <t>SF_27082020085203AGP</t>
+        </is>
+      </c>
+      <c r="F2" s="28" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="G2" s="14" t="inlineStr">
+      <c r="G2" s="13" t="inlineStr">
         <is>
           <t>Term</t>
         </is>
       </c>
-      <c r="H2" s="29" t="inlineStr">
+      <c r="H2" s="28" t="inlineStr">
         <is>
           <t>991,977.80</t>
         </is>
       </c>
-      <c r="I2" s="14" t="inlineStr">
+      <c r="I2" s="13" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="J2" s="14" t="inlineStr">
+      <c r="J2" s="13" t="inlineStr">
         <is>
           <t>26-Jun-2018</t>
         </is>
       </c>
-      <c r="K2" s="14" t="inlineStr">
+      <c r="K2" s="13" t="inlineStr">
         <is>
           <t>27-Jun-2018</t>
         </is>
       </c>
-      <c r="L2" s="14" t="inlineStr">
+      <c r="L2" s="13" t="inlineStr">
         <is>
           <t>28-Jun-2038</t>
         </is>
       </c>
-      <c r="M2" s="14" t="inlineStr">
+      <c r="M2" s="13" t="inlineStr">
         <is>
           <t>28-Jun-2038</t>
         </is>
       </c>
       <c r="N2" s="1" t="inlineStr">
         <is>
-          <t>LENDING</t>
-        </is>
-      </c>
-      <c r="O2" s="29" t="inlineStr">
+          <t>AGENCY</t>
+        </is>
+      </c>
+      <c r="O2" s="28" t="inlineStr">
         <is>
           <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
-      <c r="P2" s="29" t="inlineStr">
+      <c r="P2" s="28" t="inlineStr">
         <is>
           <t>Loan</t>
         </is>
       </c>
-      <c r="Q2" s="29" t="inlineStr">
+      <c r="Q2" s="28" t="inlineStr">
         <is>
           <t>FLOAT</t>
         </is>
       </c>
-      <c r="R2" s="14" t="inlineStr">
+      <c r="R2" s="13" t="inlineStr">
         <is>
           <t>Working Capital</t>
         </is>
       </c>
-      <c r="S2" s="14" t="inlineStr">
+      <c r="S2" s="13" t="inlineStr">
         <is>
           <t>FLOAT</t>
         </is>
       </c>
-      <c r="T2" s="14" t="inlineStr">
+      <c r="T2" s="13" t="inlineStr">
         <is>
           <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
-      <c r="U2" s="14" t="inlineStr">
+      <c r="U2" s="13" t="inlineStr">
         <is>
           <t>Sydney, NSW,Australia</t>
         </is>
       </c>
-      <c r="V2" s="1" t="inlineStr">
+      <c r="V2" s="37" t="inlineStr">
         <is>
           <t>BE Pty Ltd 08202066</t>
         </is>
       </c>
-      <c r="W2" s="14" t="inlineStr">
+      <c r="W2" s="13" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="X2" s="14" t="inlineStr">
+      <c r="X2" s="13" t="inlineStr">
         <is>
           <t>FLOAT</t>
         </is>
       </c>
-      <c r="Y2" s="14" t="inlineStr">
+      <c r="Y2" s="13" t="inlineStr">
         <is>
           <t>ELLIOT</t>
         </is>
       </c>
-      <c r="Z2" s="14" t="inlineStr">
+      <c r="Z2" s="13" t="inlineStr">
         <is>
           <t>100.000000%</t>
         </is>
       </c>
-      <c r="AA2" s="14" t="inlineStr">
+      <c r="AA2" s="13" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="AB2" s="14" t="inlineStr">
+      <c r="AB2" s="13" t="inlineStr">
         <is>
           <t>FLOAT</t>
         </is>
       </c>
     </row>
-    <row r="3" customFormat="1" s="14">
-      <c r="A3" s="14" t="inlineStr">
+    <row r="3" customFormat="1" s="13">
+      <c r="A3" s="13" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="B3" s="14" t="inlineStr">
+      <c r="B3" s="13" t="inlineStr">
         <is>
           <t>CBA_UAT_02</t>
         </is>
       </c>
-      <c r="C3" s="14" t="inlineStr">
+      <c r="C3" s="13" t="inlineStr">
         <is>
           <t>GF_</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>UAT2_26082020103334</t>
+          <t>UAT2_27082020084411</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>GF_08102019113812UHP</t>
-        </is>
-      </c>
-      <c r="F3" s="29" t="inlineStr">
+          <t>GF_27082020085831GAV</t>
+        </is>
+      </c>
+      <c r="F3" s="28" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="G3" s="14" t="inlineStr">
+      <c r="G3" s="13" t="inlineStr">
         <is>
           <t>Term</t>
         </is>
       </c>
-      <c r="H3" s="29" t="inlineStr">
+      <c r="H3" s="28" t="inlineStr">
         <is>
           <t>979,383.39</t>
         </is>
       </c>
-      <c r="I3" s="14" t="inlineStr">
+      <c r="I3" s="13" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="J3" s="14" t="inlineStr">
+      <c r="J3" s="13" t="inlineStr">
         <is>
           <t>26-Jun-2018</t>
         </is>
       </c>
-      <c r="K3" s="14" t="inlineStr">
+      <c r="K3" s="13" t="inlineStr">
         <is>
           <t>27-Jun-2018</t>
         </is>
       </c>
-      <c r="L3" s="14" t="inlineStr">
+      <c r="L3" s="13" t="inlineStr">
         <is>
           <t>27-Jun-2038</t>
         </is>
       </c>
-      <c r="M3" s="14" t="inlineStr">
+      <c r="M3" s="13" t="inlineStr">
         <is>
           <t>27-Jun-2038</t>
         </is>
       </c>
       <c r="N3" s="1" t="inlineStr">
         <is>
-          <t>LENDING</t>
-        </is>
-      </c>
-      <c r="O3" s="29" t="inlineStr">
+          <t>AGENCY</t>
+        </is>
+      </c>
+      <c r="O3" s="28" t="inlineStr">
         <is>
           <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
-      <c r="P3" s="29" t="inlineStr">
+      <c r="P3" s="28" t="inlineStr">
         <is>
           <t>Loan</t>
         </is>
       </c>
-      <c r="Q3" s="29" t="inlineStr">
+      <c r="Q3" s="28" t="inlineStr">
         <is>
           <t>FLOAT</t>
         </is>
       </c>
-      <c r="R3" s="14" t="inlineStr">
+      <c r="R3" s="13" t="inlineStr">
         <is>
           <t>Working Capital</t>
         </is>
       </c>
-      <c r="S3" s="14" t="inlineStr">
+      <c r="S3" s="13" t="inlineStr">
         <is>
           <t>FLOAT</t>
         </is>
       </c>
-      <c r="T3" s="14" t="inlineStr">
+      <c r="T3" s="13" t="inlineStr">
         <is>
           <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
-      <c r="U3" s="14" t="inlineStr">
+      <c r="U3" s="13" t="inlineStr">
         <is>
           <t>Sydney, NSW,Australia</t>
         </is>
       </c>
-      <c r="V3" s="1" t="inlineStr">
+      <c r="V3" s="37" t="inlineStr">
         <is>
           <t>BE Pty Ltd 08202066</t>
         </is>
       </c>
-      <c r="W3" s="14" t="inlineStr">
+      <c r="W3" s="13" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="X3" s="14" t="inlineStr">
+      <c r="X3" s="13" t="inlineStr">
         <is>
           <t>FLOAT</t>
         </is>
       </c>
-      <c r="Y3" s="14" t="inlineStr">
+      <c r="Y3" s="13" t="inlineStr">
         <is>
           <t>ELLIOT</t>
         </is>
       </c>
-      <c r="Z3" s="14" t="inlineStr">
+      <c r="Z3" s="13" t="inlineStr">
         <is>
           <t>100.000000%</t>
         </is>
       </c>
-      <c r="AA3" s="14" t="inlineStr">
+      <c r="AA3" s="13" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="AB3" s="14" t="inlineStr">
+      <c r="AB3" s="13" t="inlineStr">
         <is>
           <t>FLOAT</t>
         </is>
       </c>
     </row>
-    <row r="4" customFormat="1" s="14">
-      <c r="A4" s="14" t="inlineStr">
+    <row r="4" customFormat="1" s="13">
+      <c r="A4" s="13" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="B4" s="14" t="inlineStr">
+      <c r="B4" s="13" t="inlineStr">
         <is>
           <t>CBA_UAT_02</t>
         </is>
       </c>
-      <c r="C4" s="14" t="inlineStr">
+      <c r="C4" s="13" t="inlineStr">
         <is>
           <t>WF_</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>UAT2_26082020103334</t>
+          <t>UAT2_27082020084411</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr">
@@ -3807,117 +3805,117 @@
           <t>WF_08102019114236LYB</t>
         </is>
       </c>
-      <c r="F4" s="29" t="inlineStr">
+      <c r="F4" s="28" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="G4" s="14" t="inlineStr">
+      <c r="G4" s="13" t="inlineStr">
         <is>
           <t>Term</t>
         </is>
       </c>
-      <c r="H4" s="29" t="inlineStr">
+      <c r="H4" s="28" t="inlineStr">
         <is>
           <t>2,479,944.52</t>
         </is>
       </c>
-      <c r="I4" s="14" t="inlineStr">
+      <c r="I4" s="13" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="J4" s="14" t="inlineStr">
+      <c r="J4" s="13" t="inlineStr">
         <is>
           <t>26-Jun-2018</t>
         </is>
       </c>
-      <c r="K4" s="14" t="inlineStr">
+      <c r="K4" s="13" t="inlineStr">
         <is>
           <t>27-Jun-2018</t>
         </is>
       </c>
-      <c r="L4" s="14" t="inlineStr">
+      <c r="L4" s="13" t="inlineStr">
         <is>
           <t>28-Jun-2038</t>
         </is>
       </c>
-      <c r="M4" s="14" t="inlineStr">
+      <c r="M4" s="13" t="inlineStr">
         <is>
           <t>28-Jun-2038</t>
         </is>
       </c>
       <c r="N4" s="1" t="inlineStr">
         <is>
-          <t>LENDING</t>
-        </is>
-      </c>
-      <c r="O4" s="29" t="inlineStr">
+          <t>AGENCY</t>
+        </is>
+      </c>
+      <c r="O4" s="28" t="inlineStr">
         <is>
           <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
-      <c r="P4" s="29" t="inlineStr">
+      <c r="P4" s="28" t="inlineStr">
         <is>
           <t>Loan</t>
         </is>
       </c>
-      <c r="Q4" s="29" t="inlineStr">
+      <c r="Q4" s="28" t="inlineStr">
         <is>
           <t>FLOAT</t>
         </is>
       </c>
-      <c r="R4" s="14" t="inlineStr">
+      <c r="R4" s="13" t="inlineStr">
         <is>
           <t>Working Capital</t>
         </is>
       </c>
-      <c r="S4" s="14" t="inlineStr">
+      <c r="S4" s="13" t="inlineStr">
         <is>
           <t>FLOAT</t>
         </is>
       </c>
-      <c r="T4" s="14" t="inlineStr">
+      <c r="T4" s="13" t="inlineStr">
         <is>
           <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
-      <c r="U4" s="14" t="inlineStr">
+      <c r="U4" s="13" t="inlineStr">
         <is>
           <t>Sydney, NSW,Australia</t>
         </is>
       </c>
-      <c r="V4" s="1" t="inlineStr">
+      <c r="V4" s="37" t="inlineStr">
         <is>
           <t>BE Pty Ltd 08202066</t>
         </is>
       </c>
-      <c r="W4" s="14" t="inlineStr">
+      <c r="W4" s="13" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="X4" s="14" t="inlineStr">
+      <c r="X4" s="13" t="inlineStr">
         <is>
           <t>FLOAT</t>
         </is>
       </c>
-      <c r="Y4" s="14" t="inlineStr">
+      <c r="Y4" s="13" t="inlineStr">
         <is>
           <t>ELLIOT</t>
         </is>
       </c>
-      <c r="Z4" s="14" t="inlineStr">
+      <c r="Z4" s="13" t="inlineStr">
         <is>
           <t>100.000000%</t>
         </is>
       </c>
-      <c r="AA4" s="14" t="inlineStr">
+      <c r="AA4" s="13" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="AB4" s="14" t="inlineStr">
+      <c r="AB4" s="13" t="inlineStr">
         <is>
           <t>FLOAT</t>
         </is>
@@ -3956,72 +3954,72 @@
     <col width="14.5703125" customWidth="1" style="1" min="10" max="10"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" s="30">
-      <c r="A1" s="31" t="inlineStr">
+    <row r="1" customFormat="1" s="29">
+      <c r="A1" s="30" t="inlineStr">
         <is>
           <t>rowid</t>
         </is>
       </c>
-      <c r="B1" s="31" t="inlineStr">
+      <c r="B1" s="30" t="inlineStr">
         <is>
           <t>Test_Case</t>
         </is>
       </c>
-      <c r="C1" s="32" t="inlineStr">
+      <c r="C1" s="31" t="inlineStr">
         <is>
           <t>Facility_Name</t>
         </is>
       </c>
-      <c r="D1" s="30" t="inlineStr">
+      <c r="D1" s="29" t="inlineStr">
         <is>
           <t>Interest_AddItem</t>
         </is>
       </c>
-      <c r="E1" s="30" t="inlineStr">
+      <c r="E1" s="29" t="inlineStr">
         <is>
           <t>Interest_OptionName</t>
         </is>
       </c>
-      <c r="F1" s="30" t="inlineStr">
+      <c r="F1" s="29" t="inlineStr">
         <is>
           <t>Interest_RateBasis</t>
         </is>
       </c>
-      <c r="G1" s="30" t="inlineStr">
+      <c r="G1" s="29" t="inlineStr">
         <is>
           <t>Interest_SpreadValue</t>
         </is>
       </c>
-      <c r="H1" s="30" t="inlineStr">
+      <c r="H1" s="29" t="inlineStr">
         <is>
           <t>Interest_BaseRateCode</t>
         </is>
       </c>
-      <c r="I1" s="30" t="inlineStr">
+      <c r="I1" s="29" t="inlineStr">
         <is>
           <t>Penalty_Spread</t>
         </is>
       </c>
-      <c r="J1" s="30" t="inlineStr">
+      <c r="J1" s="29" t="inlineStr">
         <is>
           <t>Penalty_Status</t>
         </is>
       </c>
     </row>
     <row r="2" customFormat="1" s="1">
-      <c r="A2" s="14" t="inlineStr">
+      <c r="A2" s="13" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="B2" s="14" t="inlineStr">
+      <c r="B2" s="13" t="inlineStr">
         <is>
           <t>CBA_UAT_02</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>SF_26082020082952PCL</t>
+          <t>SF_27082020085203AGP</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
@@ -4029,7 +4027,7 @@
           <t>Option</t>
         </is>
       </c>
-      <c r="E2" s="29" t="inlineStr">
+      <c r="E2" s="28" t="inlineStr">
         <is>
           <t>Fixed Rate Option</t>
         </is>
@@ -4039,7 +4037,7 @@
           <t>Actual/365</t>
         </is>
       </c>
-      <c r="G2" s="29" t="inlineStr">
+      <c r="G2" s="28" t="inlineStr">
         <is>
           <t>1.34</t>
         </is>
@@ -4049,7 +4047,7 @@
           <t>FIX</t>
         </is>
       </c>
-      <c r="I2" s="33" t="inlineStr">
+      <c r="I2" s="32" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -4061,19 +4059,19 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="14" t="inlineStr">
+      <c r="A3" s="13" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="B3" s="14" t="inlineStr">
+      <c r="B3" s="13" t="inlineStr">
         <is>
           <t>CBA_UAT_02</t>
         </is>
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>GF_08102019113812UHP</t>
+          <t>GF_27082020085831GAV</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
@@ -4081,7 +4079,7 @@
           <t>Option</t>
         </is>
       </c>
-      <c r="E3" s="29" t="inlineStr">
+      <c r="E3" s="28" t="inlineStr">
         <is>
           <t>Fixed Rate Option</t>
         </is>
@@ -4091,7 +4089,7 @@
           <t>Actual/365</t>
         </is>
       </c>
-      <c r="G3" s="29" t="inlineStr">
+      <c r="G3" s="28" t="inlineStr">
         <is>
           <t>1.27</t>
         </is>
@@ -4101,7 +4099,7 @@
           <t>FIX</t>
         </is>
       </c>
-      <c r="I3" s="33" t="inlineStr">
+      <c r="I3" s="32" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -4113,12 +4111,12 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="14" t="inlineStr">
+      <c r="A4" s="13" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="B4" s="14" t="inlineStr">
+      <c r="B4" s="13" t="inlineStr">
         <is>
           <t>CBA_UAT_02</t>
         </is>
@@ -4133,7 +4131,7 @@
           <t>Option</t>
         </is>
       </c>
-      <c r="E4" s="29" t="inlineStr">
+      <c r="E4" s="28" t="inlineStr">
         <is>
           <t>Fixed Rate Option</t>
         </is>
@@ -4143,7 +4141,7 @@
           <t>Actual/365</t>
         </is>
       </c>
-      <c r="G4" s="29" t="inlineStr">
+      <c r="G4" s="28" t="inlineStr">
         <is>
           <t>1.34</t>
         </is>
@@ -4153,7 +4151,7 @@
           <t>FIX</t>
         </is>
       </c>
-      <c r="I4" s="33" t="inlineStr">
+      <c r="I4" s="32" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -4165,7 +4163,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="I5" s="33" t="n"/>
+      <c r="I5" s="32" t="n"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
@@ -4182,8 +4180,8 @@
   </sheetPr>
   <dimension ref="A1:AX5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -4217,27 +4215,27 @@
           <t>Test_Case</t>
         </is>
       </c>
-      <c r="C1" s="21" t="inlineStr">
+      <c r="C1" s="20" t="inlineStr">
         <is>
           <t>Deal_Name</t>
         </is>
       </c>
-      <c r="D1" s="21" t="inlineStr">
+      <c r="D1" s="20" t="inlineStr">
         <is>
           <t>Facility_Name</t>
         </is>
       </c>
-      <c r="E1" s="21" t="inlineStr">
+      <c r="E1" s="20" t="inlineStr">
         <is>
           <t>Loan_Alias</t>
         </is>
       </c>
-      <c r="F1" s="21" t="inlineStr">
+      <c r="F1" s="20" t="inlineStr">
         <is>
           <t>Borrower_Name</t>
         </is>
       </c>
-      <c r="G1" s="21" t="inlineStr">
+      <c r="G1" s="20" t="inlineStr">
         <is>
           <t>Pricing_Option</t>
         </is>
@@ -4282,12 +4280,12 @@
           <t>Loan_BorrowerBaseRate</t>
         </is>
       </c>
-      <c r="P1" s="21" t="inlineStr">
+      <c r="P1" s="20" t="inlineStr">
         <is>
           <t>Remittance_Description</t>
         </is>
       </c>
-      <c r="Q1" s="21" t="inlineStr">
+      <c r="Q1" s="20" t="inlineStr">
         <is>
           <t>Remittance_Instruction</t>
         </is>
@@ -4306,12 +4304,12 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>UAT2_26082020103334</t>
+          <t>UAT2_27082020084411</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>SF_26082020082952PCL</t>
+          <t>SF_27082020085203AGP</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
@@ -4334,15 +4332,17 @@
           <t>Loan</t>
         </is>
       </c>
-      <c r="I2" s="37" t="n">
-        <v>0.0413</v>
+      <c r="I2" s="36" t="inlineStr">
+        <is>
+          <t>1.34</t>
+        </is>
       </c>
       <c r="J2" s="1" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="K2" s="29" t="inlineStr">
+      <c r="K2" s="28" t="inlineStr">
         <is>
           <t>991,977.80</t>
         </is>
@@ -4446,12 +4446,12 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>UAT2_26082020103334</t>
+          <t>UAT2_27082020084411</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>GF_08102019113812UHP</t>
+          <t>GF_27082020085831GAV</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
@@ -4474,15 +4474,17 @@
           <t>Loan</t>
         </is>
       </c>
-      <c r="I3" s="37" t="n">
-        <v>0.0413</v>
+      <c r="I3" s="36" t="inlineStr">
+        <is>
+          <t>1.27</t>
+        </is>
       </c>
       <c r="J3" s="1" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="K3" s="29" t="inlineStr">
+      <c r="K3" s="28" t="inlineStr">
         <is>
           <t>979,383.39</t>
         </is>
@@ -4586,7 +4588,7 @@
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>UAT2_26082020103334</t>
+          <t>UAT2_27082020084411</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
@@ -4614,7 +4616,7 @@
           <t>Loan</t>
         </is>
       </c>
-      <c r="I4" s="38" t="n">
+      <c r="I4" s="36" t="n">
         <v>0.0413</v>
       </c>
       <c r="J4" s="1" t="inlineStr">
@@ -4622,7 +4624,7 @@
           <t>AUD</t>
         </is>
       </c>
-      <c r="K4" s="29" t="inlineStr">
+      <c r="K4" s="28" t="inlineStr">
         <is>
           <t>2,479,944.52</t>
         </is>
@@ -4716,7 +4718,7 @@
     <row r="5">
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>UAT2_26082020103334</t>
+          <t>UAT2_27082020084411</t>
         </is>
       </c>
       <c r="F5" s="1" t="inlineStr">
@@ -4782,37 +4784,37 @@
           <t>Test_Case</t>
         </is>
       </c>
-      <c r="C1" s="21" t="inlineStr">
+      <c r="C1" s="20" t="inlineStr">
         <is>
           <t>Deal_Name</t>
         </is>
       </c>
-      <c r="D1" s="21" t="inlineStr">
+      <c r="D1" s="20" t="inlineStr">
         <is>
           <t>Facility_Name</t>
         </is>
       </c>
-      <c r="E1" s="21" t="inlineStr">
+      <c r="E1" s="20" t="inlineStr">
         <is>
           <t>Loan_Alias</t>
         </is>
       </c>
-      <c r="F1" s="21" t="inlineStr">
+      <c r="F1" s="20" t="inlineStr">
         <is>
           <t>Pricing_Option</t>
         </is>
       </c>
-      <c r="G1" s="21" t="inlineStr">
+      <c r="G1" s="20" t="inlineStr">
         <is>
           <t>Borrower_Name</t>
         </is>
       </c>
-      <c r="H1" s="21" t="inlineStr">
+      <c r="H1" s="20" t="inlineStr">
         <is>
           <t>Remittance_Description</t>
         </is>
       </c>
-      <c r="I1" s="21" t="inlineStr">
+      <c r="I1" s="20" t="inlineStr">
         <is>
           <t>Remittance_Instruction</t>
         </is>
@@ -4876,12 +4878,12 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>UAT2_26082020103334</t>
+          <t>UAT2_27082020084411</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>SF_26082020082952PCL</t>
+          <t>SF_27082020085203AGP</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
@@ -4919,7 +4921,7 @@
           <t>Flex Schedule</t>
         </is>
       </c>
-      <c r="L2" s="34" t="inlineStr">
+      <c r="L2" s="33" t="inlineStr">
         <is>
           <t>18,432.06</t>
         </is>
@@ -4968,12 +4970,12 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>UAT2_26082020103334</t>
+          <t>UAT2_27082020084411</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>GF_08102019113812UHP</t>
+          <t>GF_27082020085831GAV</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
@@ -5011,7 +5013,7 @@
           <t>Flex Schedule</t>
         </is>
       </c>
-      <c r="L3" s="35" t="inlineStr">
+      <c r="L3" s="34" t="inlineStr">
         <is>
           <t>30,144.06</t>
         </is>
@@ -5026,7 +5028,7 @@
           <t>2</t>
         </is>
       </c>
-      <c r="O3" s="35" t="inlineStr">
+      <c r="O3" s="34" t="inlineStr">
         <is>
           <t>958,469.15</t>
         </is>
@@ -5060,7 +5062,7 @@
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>UAT2_26082020103334</t>
+          <t>UAT2_27082020084411</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
@@ -5103,7 +5105,7 @@
           <t>Flex Schedule</t>
         </is>
       </c>
-      <c r="L4" s="35" t="inlineStr">
+      <c r="L4" s="34" t="inlineStr">
         <is>
           <t>40,080.14</t>
         </is>
@@ -5122,7 +5124,7 @@
     <row r="5">
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>UAT2_26082020103334</t>
+          <t>UAT2_27082020084411</t>
         </is>
       </c>
       <c r="G5" s="1" t="inlineStr">

</xml_diff>

<commit_message>
GDE-6850 - Update 02Repayments.robot, Cashflow.robot, RepaymentPaperClip_Notebook.robot
</commit_message>
<xml_diff>
--- a/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT02.xlsx
+++ b/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT02.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{2115B222-0EDF-409D-A4CC-649096533D6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\CBAUATDeal_DataSet\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525FB5F8-56C1-4AE0-B1BD-5FC79071AA8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3105" yWindow="2265" windowWidth="21600" windowHeight="11385" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -17,12 +22,11 @@
     <sheet name="UAT02_Runbook" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="I1:P12"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="487">
   <si>
     <t>rowid</t>
   </si>
@@ -1466,12 +1470,6 @@
   </si>
   <si>
     <t>18,432.06</t>
-  </si>
-  <si>
-    <t>983,759.85</t>
-  </si>
-  <si>
-    <t>4,007.27</t>
   </si>
   <si>
     <t>01-Feb-2019</t>
@@ -4772,7 +4770,7 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4896,14 +4894,14 @@
       <c r="N2" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="33">
+        <v>983764.29</v>
+      </c>
+      <c r="P2" s="33">
+        <v>4007.29</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>480</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>482</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>41</v>
@@ -4944,7 +4942,7 @@
         <v>478</v>
       </c>
       <c r="L3" s="34" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>41</v>
@@ -4953,13 +4951,13 @@
         <v>397</v>
       </c>
       <c r="O3" s="34" t="s">
+        <v>482</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>484</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>486</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>41</v>
@@ -5000,13 +4998,13 @@
         <v>478</v>
       </c>
       <c r="L4" s="34" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>41</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>